<commit_message>
made a lot of progress
</commit_message>
<xml_diff>
--- a/bercot/time_sheet.xlsx
+++ b/bercot/time_sheet.xlsx
@@ -132,16 +132,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -168,6 +165,23 @@
       </c>
       <c r="C3" s="2"/>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>42918</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>42918</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.388888888888889</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
logic is done for Bercot's ANF parser
</commit_message>
<xml_diff>
--- a/bercot/time_sheet.xlsx
+++ b/bercot/time_sheet.xlsx
@@ -102,8 +102,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -132,54 +136,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>42915</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>42917</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>42918</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>42918</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>0.388888888888889</v>
+      <c r="B5" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>42920</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.28125</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0.338888888888889</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>42920</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0.368055555555556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error messages show up in HTML, some basic prettying up completed
</commit_message>
<xml_diff>
--- a/bercot/time_sheet.xlsx
+++ b/bercot/time_sheet.xlsx
@@ -136,18 +136,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -198,19 +198,33 @@
       <c r="A6" s="2" t="n">
         <v>42920</v>
       </c>
-      <c r="C6" s="3" t="n">
-        <v>0.28125</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>0.338888888888889</v>
-      </c>
+      <c r="B6" s="0" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>42920</v>
       </c>
-      <c r="C7" s="3" t="n">
-        <v>0.368055555555556</v>
+      <c r="B7" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>42930</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0.149305555555556</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <f aca="false">SUM(B2:B15)</f>
+        <v>10.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
splits quotes on { now, updated error notes in index.html
</commit_message>
<xml_diff>
--- a/bercot/time_sheet.xlsx
+++ b/bercot/time_sheet.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Time</t>
+    <t xml:space="preserve">Time (hrs)</t>
   </si>
 </sst>
 </file>
@@ -139,15 +139,13 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -217,14 +215,30 @@
       <c r="A8" s="2" t="n">
         <v>42930</v>
       </c>
-      <c r="C8" s="3" t="n">
-        <v>0.149305555555556</v>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>42937</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="3" t="n">
+        <v>0.0763888888888889</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <f aca="false">SUM(B2:B15)</f>
-        <v>10.03</v>
+        <v>12.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made final tweaks David wanted
</commit_message>
<xml_diff>
--- a/bercot/time_sheet.xlsx
+++ b/bercot/time_sheet.xlsx
@@ -139,13 +139,15 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -231,14 +233,27 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="3" t="n">
-        <v>0.0763888888888889</v>
-      </c>
+      <c r="A10" s="2" t="n">
+        <v>42937</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>42940</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <f aca="false">SUM(B2:B15)</f>
-        <v>12.69</v>
+        <v>13.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
misc. drafts and updates
</commit_message>
<xml_diff>
--- a/bercot/time_sheet.xlsx
+++ b/bercot/time_sheet.xlsx
@@ -363,7 +363,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -512,13 +512,13 @@
         <v>43415</v>
       </c>
       <c r="B13">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18">
         <f>SUM(B2:B15)</f>
-        <v>17.04</v>
+        <v>17.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>